<commit_message>
version 1.1 en desarrollo
</commit_message>
<xml_diff>
--- a/core/static/core/plantilla_clientes.xlsx
+++ b/core/static/core/plantilla_clientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoreno\CascadeProjects\crea_online_crm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoreno\CascadeProjects\crea_online_crm\core\static\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDD96742-4A47-42FC-9B68-A34797E0A98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC65DD68-1720-4B67-AF71-FCB790495875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8038B97-1EF9-4614-84F2-21A8FC2ACB34}"/>
   </bookViews>
@@ -36,47 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
-  <si>
-    <t xml:space="preserve">FECHA CESION </t>
-  </si>
-  <si>
-    <t>FECHA ACT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOCUMENTO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFERENCIA </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>CC</t>
   </si>
   <si>
-    <t>NOMBRE COMPLETO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIUDAD </t>
-  </si>
-  <si>
-    <t>DIAS MORA ORIGINADOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIAS MORA CASO SAS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL DIAS MORA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AÑOS MORA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRINCIPAL </t>
-  </si>
-  <si>
-    <t>DEUDA PRINCIPAL K</t>
-  </si>
-  <si>
     <t>INTERESES</t>
   </si>
   <si>
@@ -86,27 +50,6 @@
     <t>SEGURO</t>
   </si>
   <si>
-    <t>OTROS CARGOS</t>
-  </si>
-  <si>
-    <t>TOTAL PAGADO</t>
-  </si>
-  <si>
-    <t>DCTO PAGO CONTADO 50%</t>
-  </si>
-  <si>
-    <t>DCTO PAGO CONTADO 70% MAX. 30%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEUDA TOTAL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELEFONO CELULAR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAIL </t>
-  </si>
-  <si>
     <t>CELULAR_1</t>
   </si>
   <si>
@@ -116,39 +59,6 @@
     <t>CELULAR_3</t>
   </si>
   <si>
-    <t>CELULAR_4</t>
-  </si>
-  <si>
-    <t>CELULAR_5</t>
-  </si>
-  <si>
-    <t>DIRECCION 1</t>
-  </si>
-  <si>
-    <t>DIRECCION 2</t>
-  </si>
-  <si>
-    <t>DIRECCION 3</t>
-  </si>
-  <si>
-    <t>EMAIL 1</t>
-  </si>
-  <si>
-    <t>EMAIL 2</t>
-  </si>
-  <si>
-    <t>EMAIL 3</t>
-  </si>
-  <si>
-    <t>TELEFONO 1</t>
-  </si>
-  <si>
-    <t>TELEFONO 2</t>
-  </si>
-  <si>
-    <t>TELEFONO 3</t>
-  </si>
-  <si>
     <t>Yheimit Zulay Ortiz Sanchez</t>
   </si>
   <si>
@@ -165,6 +75,87 @@
   </si>
   <si>
     <t>KR 11 12 16</t>
+  </si>
+  <si>
+    <t>FECHA_ACT</t>
+  </si>
+  <si>
+    <t>NOMBRE_COMPLETO</t>
+  </si>
+  <si>
+    <t>DIAS_MORA_ORIGINADOR</t>
+  </si>
+  <si>
+    <t>DEUDA_PRINCIPAL_K</t>
+  </si>
+  <si>
+    <t>OTROS_CARGOS</t>
+  </si>
+  <si>
+    <t>TOTAL_PAGADO</t>
+  </si>
+  <si>
+    <t>DCTO_PAGO_CONTADO_50%</t>
+  </si>
+  <si>
+    <t>DIRECCION_1</t>
+  </si>
+  <si>
+    <t>DIRECCION_2</t>
+  </si>
+  <si>
+    <t>DIRECCION_3</t>
+  </si>
+  <si>
+    <t>EMAIL_1</t>
+  </si>
+  <si>
+    <t>EMAIL_2</t>
+  </si>
+  <si>
+    <t>TELEFONO_1</t>
+  </si>
+  <si>
+    <t>TELEFONO_2</t>
+  </si>
+  <si>
+    <t>FECHA_CESION</t>
+  </si>
+  <si>
+    <t>DOCUMENTO</t>
+  </si>
+  <si>
+    <t>REFERENCIA</t>
+  </si>
+  <si>
+    <t>CIUDAD</t>
+  </si>
+  <si>
+    <t>DIAS_MORA_CASO_SAS</t>
+  </si>
+  <si>
+    <t>TOTAL_DIAS_MORA</t>
+  </si>
+  <si>
+    <t>AÑOS_MORA</t>
+  </si>
+  <si>
+    <t>PRINCIPAL</t>
+  </si>
+  <si>
+    <t>DCTO_PAGO_CONTADO_70%_MAX_30%</t>
+  </si>
+  <si>
+    <t>DEUDA_TOTAL</t>
+  </si>
+  <si>
+    <t>TELEFONO_CELULAR</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TIPO_DOCUMENTO</t>
   </si>
 </sst>
 </file>
@@ -254,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -262,35 +253,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -636,134 +609,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E005606-4D0E-41A7-83D1-ABE7B15CC93E}">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>45800</v>
       </c>
-      <c r="B2" s="4">
-        <f t="shared" ref="B2" ca="1" si="0">+TODAY()</f>
+      <c r="B2" s="3">
         <v>45804</v>
       </c>
       <c r="C2">
@@ -773,110 +737,90 @@
         <v>2830089787</v>
       </c>
       <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2086</v>
+      </c>
+      <c r="I2" s="4">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>1100973028</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="5">
-        <v>2086</v>
-      </c>
-      <c r="J2" s="5">
-        <f t="shared" ref="J2" ca="1" si="1">+_xlfn.DAYS(B2,A2)</f>
-        <v>4</v>
-      </c>
-      <c r="K2" s="5">
-        <f t="shared" ref="K2" ca="1" si="2">+I2+J2</f>
+      <c r="J2" s="4">
         <v>2090</v>
       </c>
+      <c r="K2" s="4">
+        <v>5.8055555555555554</v>
+      </c>
       <c r="L2" s="5">
-        <f t="shared" ref="L2" ca="1" si="3">+K2/360</f>
-        <v>5.8055555555555554</v>
+        <v>250000</v>
       </c>
       <c r="M2" s="6">
         <v>250000</v>
       </c>
       <c r="N2" s="7">
-        <v>250000</v>
-      </c>
-      <c r="O2" s="8">
         <v>669997.88</v>
       </c>
-      <c r="P2" s="8">
+      <c r="O2" s="7">
         <v>72000</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="P2" s="7">
         <v>2266.0700000000002</v>
       </c>
-      <c r="R2" s="8">
-        <v>51759.98999999994</v>
+      <c r="Q2" s="7">
+        <v>51759.989999999903</v>
+      </c>
+      <c r="R2" s="7">
+        <v>0</v>
       </c>
       <c r="S2" s="8">
+        <v>524000</v>
+      </c>
+      <c r="T2" s="9">
+        <v>733000</v>
+      </c>
+      <c r="U2" s="10">
+        <v>1046023.94</v>
+      </c>
+      <c r="V2">
+        <v>3024484416</v>
+      </c>
+      <c r="W2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2">
         <v>0</v>
-      </c>
-      <c r="T2" s="9">
-        <f>ROUNDUP((V2/2),-3)</f>
-        <v>524000</v>
-      </c>
-      <c r="U2" s="10">
-        <f>+ROUNDUP((V2*70%),-3)</f>
-        <v>733000</v>
-      </c>
-      <c r="V2" s="11">
-        <v>1046023.94</v>
-      </c>
-      <c r="W2">
-        <v>3024484416</v>
-      </c>
-      <c r="X2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>40</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
+      <c r="AA2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
       </c>
       <c r="AC2">
         <v>0</v>
       </c>
-      <c r="AD2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>42</v>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
       </c>
       <c r="AF2">
         <v>0</v>
       </c>
       <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
         <v>0</v>
       </c>
     </row>

</xml_diff>